<commit_message>
Report update @ 30-Aug-2025 23:59:41
</commit_message>
<xml_diff>
--- a/aircraft/reports/aircraft-type-trends-monthly.xlsx
+++ b/aircraft/reports/aircraft-type-trends-monthly.xlsx
@@ -4362,7 +4362,7 @@
         <v>2</v>
       </c>
       <c r="G74" t="n">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="H74" t="n">
         <v>30</v>
@@ -4374,7 +4374,7 @@
         <v>26</v>
       </c>
       <c r="K74" t="n">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="L74" t="n">
         <v>24</v>
@@ -4392,7 +4392,7 @@
         <v>13</v>
       </c>
       <c r="Q74" t="n">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>